<commit_message>
updated with connection to database
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathy\Desktop\GITRepositories\mlenv_movie_success_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882DED1B-3ED5-4F35-B51F-43B37F59477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A268C9-593D-4095-A3E7-4A616628B0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18180" yWindow="456" windowWidth="15936" windowHeight="9792" xr2:uid="{D29C7B10-7CC1-4060-9C91-144D6B1716F6}"/>
+    <workbookView xWindow="-10152" yWindow="996" windowWidth="9840" windowHeight="9792" activeTab="1" xr2:uid="{D29C7B10-7CC1-4060-9C91-144D6B1716F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Comparison of Models</t>
   </si>
@@ -64,6 +65,12 @@
   </si>
   <si>
     <t>Deep Learning Final</t>
+  </si>
+  <si>
+    <t>using csv file</t>
+  </si>
+  <si>
+    <t>using database</t>
   </si>
 </sst>
 </file>
@@ -71,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +111,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54B1984-5592-402B-BAB8-B2B01318A311}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,6 +541,139 @@
         <v>0.12</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ED8D6-F80D-4AE7-A264-6CC66F409500}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>